<commit_message>
Typo sur certains libellés
</commit_message>
<xml_diff>
--- a/tools/mcas/mcas-1.0.xlsx
+++ b/tools/mcas/mcas-1.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gildas/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gildas/Documents/Codes/security/CISO/ciso-assistant-community/tools/mcas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7829C049-0FE4-384B-A693-0CE6DC5CD310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE3169B-AFFC-6648-B20D-087ADCEBFFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="19000" activeTab="1" xr2:uid="{D548BFD9-24AA-6740-B2D6-47677657AB26}"/>
   </bookViews>
@@ -1296,12 +1296,6 @@
     <t>Le déploiement de réseaux sans fil doit faire l'objet d'une analyse de risques spécifique. Les protections intrinsèques étant insuffisantes, des mesures complémentaires, validées par le SHFDS, doivent être prises dans le cadre de la défense en profondeur. En particulier, une segmentation du réseau doit être mise en place de façon à limiter â un périmètre déterminé les conséquences d’une intrusion depuis la voie radio. À défaut de mise en œuvre de mesures spécifiques, le déploiement de réseaux sans fil sur des SI manipulant des données sensibles est proscrit Sécurisation des mécanismes de commutation et de routage</t>
   </si>
   <si>
-    <t>Implanter des mécanismes de protection contre les attaques sur les</t>
-  </si>
-  <si>
-    <t>couches basses. Une attention particulière doit être apportée â l'implantation des protocoles de couches basses, de façon à se prémunir des attaques usuelles.</t>
-  </si>
-  <si>
     <t>Lorsque l’utilisation de protocoles de routage dynamiques est nécessaire, celle-ci doit s'accompagner de la mise en place d’une surveillance des annonces de routage, et de procédures permettant de réagir rapidement en cas d’incidents.</t>
   </si>
   <si>
@@ -1311,12 +1305,6 @@
     <t>Lors de la mise en place d’une session EGP avec un pair extérieur sur un média partagé, cette session doit être réalisée suivant les préconisations de l’Agence nationale de sécurité des systèmes d’information.</t>
   </si>
   <si>
-    <t>Modifier systématiquement les éléments d’authentification par défaut des</t>
-  </si>
-  <si>
-    <t>équipements et services. Les mots de passe par défaut doivent être impérativement modifiés, de même en ce qui concerne les certificats. Les dispositions nécessaires doivent être prises auprès des fournisseurs de façon à pouvoir modifier les certificats installés par défaut.</t>
-  </si>
-  <si>
     <t>Élaborer les documents d’architecture technique et fonctionnelle</t>
   </si>
   <si>
@@ -1437,36 +1425,18 @@
     <t>Les événements de sécurité de l'antivirus doivent être remontés sur un serveur central pour analyse statistique et gestion des problèmes a posteriori (exemples : serveur constamment infecté, virus détecté et non éradiqué par l'antivirus, etc.).</t>
   </si>
   <si>
-    <t>Mise à lourde la base de signatures</t>
-  </si>
-  <si>
     <t>Les mises à jour des bases antivirales et des moteurs d'antivirus doivent être déployées automatiquement sur les serveurs et les postes de travail par un dispositif prescrit par les directions, bureaux ou services informatiques, validé par le RSSI.</t>
   </si>
   <si>
-    <t>Définir et mettre en œuvre une politique de suivi et d’application des</t>
-  </si>
-  <si>
-    <t>correctifs de sécurité. Le maintien dans le temps du niveau de sécurité d’un système d’information impose une gestion organisée et adaptée des mises à jour de sécurité. Un processus de gestion des correctifs propre à chaque système ou applicatif doit être défini, et adapté suivant les contraintes et le niveau d’exposition du système.</t>
-  </si>
-  <si>
     <t>Les correctifs de sécurité des ressources informatiques locales doivent être déployés par l'équipe locale chargée des SI en s’appuyant sur les préconisations et outils proposés par les directions, bureaux ou services informatiques.</t>
   </si>
   <si>
     <t>L’ensemble des logiciels utilisés sur le système d’information doit être dans une version pour laquelle l'éditeur assure le support, et tenu à jour. En cas de défaillance du support, il convient d'en étudier l’impact et de prendre les mesures adaptées.</t>
   </si>
   <si>
-    <t>Définir et mettre en œuvre une politique de gestion et d’analyse des</t>
-  </si>
-  <si>
-    <t>journaux de traces. Une politique de gestion et d'analyse des journaux de traces des événements de sécurité est définie par le RSSI, validée par l’autorité qualifiée, et mise en œuvre. Le niveau de sécurité d’un système d’information dépend en grande partie de la capacité de ses exploitants et administrateurs à détecter les erreurs, dysfonctionnements et tentatives d’accès illicites survenant sur les éléments qui le composent.</t>
-  </si>
-  <si>
     <t>Les personnes en charge de la SSI doivent procéder, notamment via l'analyse des journaux, à la surveillance des comportements anormaux au sein du système d'information, et à la surveillance des flux d'entrée et de sortie du système d'information. Gestion des matériels informatiques fournis à l'utilisateur</t>
   </si>
   <si>
-    <t>Maîtrise des matériels,</t>
-  </si>
-  <si>
     <t>Les postes de travail - y compris dans le cas d'une location - sont fournis à l'utilisateur par l’entité, gérés et configurés sous la responsabilité de l'entité. La connexion d'équipements non maîtrisés, non administrés ou non mis à jour par l’entité (qu'il s'agisse d'ordiphones, d'équipements informatiques nomades et fixes ou de supports de stockage amovibles) sur des équipements et des réseaux professionnels est interdite.</t>
   </si>
   <si>
@@ -1476,21 +1446,12 @@
     <t>Toute perte ou vol d'une ressource d’un système d’information doit être déclarée au RSSI.</t>
   </si>
   <si>
-    <t>Déclaration des équipements nomades aptes à traiter des</t>
-  </si>
-  <si>
-    <t>informations sensibles. L’autorité d'homologation du SI valide les usages possibles des équipements nomades vis-à-vis du traitement des informations sensibles ; les usages non explicitement autorisés sont interdits.</t>
-  </si>
-  <si>
     <t>Les impressions d’informations sensibles doivent être effectuées selon une procédure prédéfinie, garantissant le contrôle de l'utilisateur, du déclenchement de l’impression jusqu’à la récupération du support imprimé.</t>
   </si>
   <si>
     <t xml:space="preserve">Les imprimantes et copieurs multifonctions sont des ressources informatiques à part entière qui doivent être gérées en tant que telles. Elles ne doivent pas pouvoir communiquer directement avec l’extérieur.  </t>
   </si>
   <si>
-    <t>Systèmes d’exploitation,</t>
-  </si>
-  <si>
     <t>Les systèmes d'exploitation déployés doivent faire l'objet d'un support valide de la part d’un éditeur ou d’un prestataire de service. Seuls les services et applications nécessaires sont installés, de façon à réduire la surface d'attaque. Une attention particulière doit être apportée aux comptes administrateurs.</t>
   </si>
   <si>
@@ -1530,9 +1491,6 @@
     <t>Dans un centre informatique, le contrôle physique des accès réseaux, l'attribution des adresses IP, le filtrage des informations et l'usage de dispositifs spécifiques (machines virtuelles, cartes d’administration à distance, etc.) font l'objet de procédures sécurisées.</t>
   </si>
   <si>
-    <t>AudiWcontrôle</t>
-  </si>
-  <si>
     <t>Le RSSI pilote des audits réguliers du système d’information relevant de sa responsabilité.</t>
   </si>
   <si>
@@ -1560,9 +1518,6 @@
     <t>Dans la mesure du possible, les données traitées par les utilisateurs doivent être stockées sur des espaces réseau, eux-mêmes sauvegardés selon les exigences des entités.</t>
   </si>
   <si>
-    <t>Sauvegarde I synchronisation des données locales</t>
-  </si>
-  <si>
     <t>PDT-SUPPR-PART</t>
   </si>
   <si>
@@ -1654,12 +1609,6 @@
   </si>
   <si>
     <t>Définition du plan ministériel de continuité d’activité des Systèmes</t>
-  </si>
-  <si>
-    <t>Suivi de la mise en œuvre du plan de continuité d'activité local des</t>
-  </si>
-  <si>
-    <t>Système d'Information (PCA des SI). Le RSSI d'une entité s’assure de la bonne mise en œuvre des dispositions prévues dans le plan de continuité d’activité des systèmes d’information.</t>
   </si>
   <si>
     <t>Mise en œuvre des dispositifs techniques et des procédures opérationnelles</t>
@@ -1888,6 +1837,57 @@
   </si>
   <si>
     <t>PDT-TEL-MINIM</t>
+  </si>
+  <si>
+    <t>Une attention particulière doit être apportée â l'implantation des protocoles de couches basses, de façon à se prémunir des attaques usuelles.</t>
+  </si>
+  <si>
+    <t>Implanter des mécanismes de protection contre les attaques sur les couches basses</t>
+  </si>
+  <si>
+    <t>Les mots de passe par défaut doivent être impérativement modifiés, de même en ce qui concerne les certificats. Les dispositions nécessaires doivent être prises auprès des fournisseurs de façon à pouvoir modifier les certificats installés par défaut.</t>
+  </si>
+  <si>
+    <t>Modifier systématiquement les éléments d’authentification par défaut des équipements et services</t>
+  </si>
+  <si>
+    <t>Audit/Contrôle</t>
+  </si>
+  <si>
+    <t>Mise à jour de la base de signatures</t>
+  </si>
+  <si>
+    <t>Une politique de gestion et d'analyse des journaux de traces des événements de sécurité est définie par le RSSI, validée par l’autorité qualifiée, et mise en œuvre. Le niveau de sécurité d’un système d’information dépend en grande partie de la capacité de ses exploitants et administrateurs à détecter les erreurs, dysfonctionnements et tentatives d’accès illicites survenant sur les éléments qui le composent.</t>
+  </si>
+  <si>
+    <t>Définir et mettre en œuvre une politique de gestion et d’analyse des journaux de traces</t>
+  </si>
+  <si>
+    <t>Le maintien dans le temps du niveau de sécurité d’un système d’information impose une gestion organisée et adaptée des mises à jour de sécurité. Un processus de gestion des correctifs propre à chaque système ou applicatif doit être défini, et adapté suivant les contraintes et le niveau d’exposition du système.</t>
+  </si>
+  <si>
+    <t>Définir et mettre en œuvre une politique de suivi et d’application des correctifs de sécurité</t>
+  </si>
+  <si>
+    <t>Maîtrise des matériels</t>
+  </si>
+  <si>
+    <t>Sauvegarde / synchronisation des données locales</t>
+  </si>
+  <si>
+    <t>L’autorité d'homologation du SI valide les usages possibles des équipements nomades vis-à-vis du traitement des informations sensibles ; les usages non explicitement autorisés sont interdits.</t>
+  </si>
+  <si>
+    <t>Déclaration des équipements nomades aptes à traiter des informations sensibles</t>
+  </si>
+  <si>
+    <t>Systèmes d’exploitation</t>
+  </si>
+  <si>
+    <t>Le RSSI d'une entité s’assure de la bonne mise en œuvre des dispositions prévues dans le plan de continuité d’activité des systèmes d’information.</t>
+  </si>
+  <si>
+    <t>Suivi de la mise en œuvre du plan de continuité d'activité local des Systèmes d'Information (PCA des SI)</t>
   </si>
 </sst>
 </file>
@@ -2414,7 +2414,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>549</v>
+        <v>532</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2478,8 +2478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F5F993-1285-4A4F-B2E7-39BB31DE6BB0}">
   <dimension ref="A1:G444"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
+      <selection activeCell="D185" sqref="D185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2688,7 +2688,7 @@
         <v>384</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>561</v>
+        <v>544</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2739,7 +2739,7 @@
         <v>50</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>562</v>
+        <v>545</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="119">
@@ -2756,7 +2756,7 @@
         <v>42</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>550</v>
+        <v>533</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2837,7 +2837,7 @@
         <v>58</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>563</v>
+        <v>546</v>
       </c>
       <c r="F21" s="12"/>
     </row>
@@ -2877,13 +2877,13 @@
         <v>2</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>599</v>
+        <v>582</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>393</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>564</v>
+        <v>547</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2934,7 +2934,7 @@
         <v>76</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>551</v>
+        <v>534</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="327" customHeight="1">
@@ -2951,7 +2951,7 @@
         <v>60</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>552</v>
+        <v>535</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2968,7 +2968,7 @@
         <v>64</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>565</v>
+        <v>548</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="102">
@@ -2985,7 +2985,7 @@
         <v>62</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>553</v>
+        <v>536</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -3038,7 +3038,7 @@
         <v>72</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>566</v>
+        <v>549</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -3066,7 +3066,7 @@
         <v>105</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>567</v>
+        <v>550</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -3100,7 +3100,7 @@
         <v>400</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>568</v>
+        <v>551</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -3188,7 +3188,7 @@
         <v>88</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>569</v>
+        <v>552</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -3239,7 +3239,7 @@
         <v>92</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>570</v>
+        <v>553</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -3301,13 +3301,13 @@
         <v>2</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>600</v>
+        <v>583</v>
       </c>
       <c r="D49" s="10" t="s">
         <v>80</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>571</v>
+        <v>554</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -3369,7 +3369,7 @@
         <v>115</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>572</v>
+        <v>555</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -3454,7 +3454,7 @@
         <v>125</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>573</v>
+        <v>556</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -3471,7 +3471,7 @@
         <v>119</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>574</v>
+        <v>557</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -3502,10 +3502,10 @@
         <v>109</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>418</v>
+        <v>589</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>419</v>
+        <v>588</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -3522,7 +3522,7 @@
         <v>127</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -3539,7 +3539,7 @@
         <v>131</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -3556,7 +3556,7 @@
         <v>129</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -3570,10 +3570,10 @@
         <v>132</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>423</v>
+        <v>591</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>424</v>
+        <v>590</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -3590,7 +3590,7 @@
         <v>111</v>
       </c>
       <c r="E66" s="10" t="s">
-        <v>575</v>
+        <v>558</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -3604,10 +3604,10 @@
         <v>106</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -3615,10 +3615,10 @@
         <v>1</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -3632,10 +3632,10 @@
         <v>140</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -3669,7 +3669,7 @@
         <v>138</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -3677,10 +3677,10 @@
         <v>1</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -3697,7 +3697,7 @@
         <v>160</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -3714,7 +3714,7 @@
         <v>141</v>
       </c>
       <c r="E74" s="10" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -3731,7 +3731,7 @@
         <v>231</v>
       </c>
       <c r="E75" s="10" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -3748,7 +3748,7 @@
         <v>221</v>
       </c>
       <c r="E76" s="10" t="s">
-        <v>576</v>
+        <v>559</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -3762,10 +3762,10 @@
         <v>195</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="E77" s="10" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -3782,7 +3782,7 @@
         <v>208</v>
       </c>
       <c r="E78" s="10" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -3796,10 +3796,10 @@
         <v>164</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="E79" s="10" t="s">
-        <v>577</v>
+        <v>560</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -3816,7 +3816,7 @@
         <v>165</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -3833,7 +3833,7 @@
         <v>148</v>
       </c>
       <c r="E81" s="10" t="s">
-        <v>578</v>
+        <v>561</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -3850,7 +3850,7 @@
         <v>233</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -3884,7 +3884,7 @@
         <v>189</v>
       </c>
       <c r="E84" s="10" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -3901,7 +3901,7 @@
         <v>167</v>
       </c>
       <c r="E85" s="10" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -3935,7 +3935,7 @@
         <v>154</v>
       </c>
       <c r="E87" s="10" t="s">
-        <v>579</v>
+        <v>562</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -3952,7 +3952,7 @@
         <v>143</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -3986,7 +3986,7 @@
         <v>223</v>
       </c>
       <c r="E90" s="10" t="s">
-        <v>580</v>
+        <v>563</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -4003,7 +4003,7 @@
         <v>150</v>
       </c>
       <c r="E91" s="10" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -4020,7 +4020,7 @@
         <v>162</v>
       </c>
       <c r="E92" s="10" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -4037,7 +4037,7 @@
         <v>196</v>
       </c>
       <c r="E93" s="10" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -4068,10 +4068,10 @@
         <v>147</v>
       </c>
       <c r="D95" s="10" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="E95" s="10" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -4088,7 +4088,7 @@
         <v>270</v>
       </c>
       <c r="E96" s="10" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -4105,7 +4105,7 @@
         <v>145</v>
       </c>
       <c r="E97" s="10" t="s">
-        <v>581</v>
+        <v>564</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -4116,13 +4116,13 @@
         <v>2</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D98" s="10" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="E98" s="10" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -4156,7 +4156,7 @@
         <v>216</v>
       </c>
       <c r="E100" s="10" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -4167,13 +4167,13 @@
         <v>2</v>
       </c>
       <c r="C101" s="10" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="D101" s="10" t="s">
         <v>214</v>
       </c>
       <c r="E101" s="10" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -4184,13 +4184,13 @@
         <v>2</v>
       </c>
       <c r="C102" s="10" t="s">
-        <v>601</v>
+        <v>584</v>
       </c>
       <c r="D102" s="10" t="s">
         <v>210</v>
       </c>
       <c r="E102" s="10" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -4201,7 +4201,7 @@
         <v>2</v>
       </c>
       <c r="C103" s="10" t="s">
-        <v>602</v>
+        <v>585</v>
       </c>
       <c r="D103" s="10" t="s">
         <v>218</v>
@@ -4218,13 +4218,13 @@
         <v>2</v>
       </c>
       <c r="C104" s="10" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="D104" s="10" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="E104" s="10" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -4241,7 +4241,7 @@
         <v>219</v>
       </c>
       <c r="E105" s="10" t="s">
-        <v>582</v>
+        <v>565</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -4258,7 +4258,7 @@
         <v>182</v>
       </c>
       <c r="E106" s="10" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="85">
@@ -4275,7 +4275,7 @@
         <v>179</v>
       </c>
       <c r="E107" s="11" t="s">
-        <v>554</v>
+        <v>537</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -4292,7 +4292,7 @@
         <v>158</v>
       </c>
       <c r="E108" s="10" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -4309,7 +4309,7 @@
         <v>207</v>
       </c>
       <c r="E109" s="10" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -4320,13 +4320,13 @@
         <v>2</v>
       </c>
       <c r="C110" s="10" t="s">
-        <v>603</v>
+        <v>586</v>
       </c>
       <c r="D110" s="10" t="s">
-        <v>465</v>
+        <v>593</v>
       </c>
       <c r="E110" s="10" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -4343,7 +4343,7 @@
         <v>177</v>
       </c>
       <c r="E111" s="10" t="s">
-        <v>555</v>
+        <v>538</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -4357,10 +4357,10 @@
         <v>170</v>
       </c>
       <c r="D112" s="10" t="s">
-        <v>467</v>
+        <v>597</v>
       </c>
       <c r="E112" s="10" t="s">
-        <v>468</v>
+        <v>596</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -4377,7 +4377,7 @@
         <v>227</v>
       </c>
       <c r="E113" s="10" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -4394,7 +4394,7 @@
         <v>174</v>
       </c>
       <c r="E114" s="10" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -4411,7 +4411,7 @@
         <v>187</v>
       </c>
       <c r="E115" s="10" t="s">
-        <v>583</v>
+        <v>566</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -4442,10 +4442,10 @@
         <v>169</v>
       </c>
       <c r="D117" s="10" t="s">
-        <v>471</v>
+        <v>595</v>
       </c>
       <c r="E117" s="10" t="s">
-        <v>472</v>
+        <v>594</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -4462,7 +4462,7 @@
         <v>229</v>
       </c>
       <c r="E118" s="10" t="s">
-        <v>584</v>
+        <v>567</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -4479,7 +4479,7 @@
         <v>204</v>
       </c>
       <c r="E119" s="10" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -4493,10 +4493,10 @@
         <v>181</v>
       </c>
       <c r="D120" s="10" t="s">
-        <v>474</v>
+        <v>598</v>
       </c>
       <c r="E120" s="10" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -4513,7 +4513,7 @@
         <v>156</v>
       </c>
       <c r="E121" s="10" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -4530,7 +4530,7 @@
         <v>225</v>
       </c>
       <c r="E122" s="10" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -4547,7 +4547,7 @@
         <v>152</v>
       </c>
       <c r="E123" s="10" t="s">
-        <v>585</v>
+        <v>568</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -4561,10 +4561,10 @@
         <v>176</v>
       </c>
       <c r="D124" s="10" t="s">
-        <v>478</v>
+        <v>601</v>
       </c>
       <c r="E124" s="10" t="s">
-        <v>479</v>
+        <v>600</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -4581,7 +4581,7 @@
         <v>272</v>
       </c>
       <c r="E125" s="10" t="s">
-        <v>586</v>
+        <v>569</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -4598,7 +4598,7 @@
         <v>191</v>
       </c>
       <c r="E126" s="10" t="s">
-        <v>480</v>
+        <v>468</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -4615,7 +4615,7 @@
         <v>193</v>
       </c>
       <c r="E127" s="10" t="s">
-        <v>481</v>
+        <v>469</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -4629,10 +4629,10 @@
         <v>242</v>
       </c>
       <c r="D128" s="10" t="s">
-        <v>482</v>
+        <v>602</v>
       </c>
       <c r="E128" s="10" t="s">
-        <v>483</v>
+        <v>470</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -4666,7 +4666,7 @@
         <v>251</v>
       </c>
       <c r="E130" s="10" t="s">
-        <v>484</v>
+        <v>471</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -4683,7 +4683,7 @@
         <v>249</v>
       </c>
       <c r="E131" s="10" t="s">
-        <v>485</v>
+        <v>472</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -4700,7 +4700,7 @@
         <v>240</v>
       </c>
       <c r="E132" s="10" t="s">
-        <v>486</v>
+        <v>473</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -4748,10 +4748,10 @@
         <v>264</v>
       </c>
       <c r="D135" s="10" t="s">
-        <v>487</v>
+        <v>474</v>
       </c>
       <c r="E135" s="10" t="s">
-        <v>488</v>
+        <v>475</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -4765,10 +4765,10 @@
         <v>258</v>
       </c>
       <c r="D136" s="10" t="s">
-        <v>489</v>
+        <v>476</v>
       </c>
       <c r="E136" s="10" t="s">
-        <v>490</v>
+        <v>477</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -4785,7 +4785,7 @@
         <v>256</v>
       </c>
       <c r="E137" s="10" t="s">
-        <v>491</v>
+        <v>478</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -4802,7 +4802,7 @@
         <v>259</v>
       </c>
       <c r="E138" s="10" t="s">
-        <v>492</v>
+        <v>479</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -4819,7 +4819,7 @@
         <v>235</v>
       </c>
       <c r="E139" s="10" t="s">
-        <v>493</v>
+        <v>480</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -4853,7 +4853,7 @@
         <v>262</v>
       </c>
       <c r="E141" s="10" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -4870,7 +4870,7 @@
         <v>265</v>
       </c>
       <c r="E142" s="10" t="s">
-        <v>495</v>
+        <v>482</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -4884,10 +4884,10 @@
         <v>261</v>
       </c>
       <c r="D143" s="10" t="s">
-        <v>496</v>
+        <v>592</v>
       </c>
       <c r="E143" s="10" t="s">
-        <v>497</v>
+        <v>483</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -4895,10 +4895,10 @@
         <v>1</v>
       </c>
       <c r="C144" s="10" t="s">
-        <v>498</v>
+        <v>484</v>
       </c>
       <c r="D144" s="10" t="s">
-        <v>499</v>
+        <v>485</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="51">
@@ -4912,10 +4912,10 @@
         <v>315</v>
       </c>
       <c r="D145" s="10" t="s">
-        <v>500</v>
+        <v>486</v>
       </c>
       <c r="E145" s="11" t="s">
-        <v>556</v>
+        <v>539</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -4929,10 +4929,10 @@
         <v>316</v>
       </c>
       <c r="D146" s="10" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="E146" s="10" t="s">
-        <v>557</v>
+        <v>540</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -4966,7 +4966,7 @@
         <v>274</v>
       </c>
       <c r="E148" s="10" t="s">
-        <v>558</v>
+        <v>541</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -4983,7 +4983,7 @@
         <v>289</v>
       </c>
       <c r="E149" s="10" t="s">
-        <v>502</v>
+        <v>488</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -5000,7 +5000,7 @@
         <v>291</v>
       </c>
       <c r="E150" s="10" t="s">
-        <v>503</v>
+        <v>489</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -5017,7 +5017,7 @@
         <v>293</v>
       </c>
       <c r="E151" s="10" t="s">
-        <v>504</v>
+        <v>490</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -5034,7 +5034,7 @@
         <v>324</v>
       </c>
       <c r="E152" s="10" t="s">
-        <v>587</v>
+        <v>570</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -5051,7 +5051,7 @@
         <v>285</v>
       </c>
       <c r="E153" s="10" t="s">
-        <v>505</v>
+        <v>491</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -5065,7 +5065,7 @@
         <v>288</v>
       </c>
       <c r="D154" s="10" t="s">
-        <v>506</v>
+        <v>599</v>
       </c>
       <c r="E154" s="10" t="s">
         <v>287</v>
@@ -5085,7 +5085,7 @@
         <v>295</v>
       </c>
       <c r="E155" s="10" t="s">
-        <v>588</v>
+        <v>571</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -5096,7 +5096,7 @@
         <v>2</v>
       </c>
       <c r="C156" s="10" t="s">
-        <v>507</v>
+        <v>492</v>
       </c>
       <c r="D156" s="10" t="s">
         <v>298</v>
@@ -5136,7 +5136,7 @@
         <v>322</v>
       </c>
       <c r="E158" s="10" t="s">
-        <v>589</v>
+        <v>572</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -5150,10 +5150,10 @@
         <v>310</v>
       </c>
       <c r="D159" s="10" t="s">
-        <v>508</v>
+        <v>493</v>
       </c>
       <c r="E159" s="10" t="s">
-        <v>509</v>
+        <v>494</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -5181,7 +5181,7 @@
         <v>2</v>
       </c>
       <c r="C161" s="10" t="s">
-        <v>510</v>
+        <v>495</v>
       </c>
       <c r="D161" s="10" t="s">
         <v>303</v>
@@ -5204,7 +5204,7 @@
         <v>304</v>
       </c>
       <c r="E162" s="10" t="s">
-        <v>511</v>
+        <v>496</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -5221,7 +5221,7 @@
         <v>308</v>
       </c>
       <c r="E163" s="10" t="s">
-        <v>512</v>
+        <v>497</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -5238,7 +5238,7 @@
         <v>306</v>
       </c>
       <c r="E164" s="10" t="s">
-        <v>590</v>
+        <v>573</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -5255,7 +5255,7 @@
         <v>313</v>
       </c>
       <c r="E165" s="10" t="s">
-        <v>513</v>
+        <v>498</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -5272,7 +5272,7 @@
         <v>311</v>
       </c>
       <c r="E166" s="10" t="s">
-        <v>514</v>
+        <v>499</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -5283,13 +5283,13 @@
         <v>2</v>
       </c>
       <c r="C167" t="s">
-        <v>604</v>
+        <v>587</v>
       </c>
       <c r="D167" s="10" t="s">
         <v>279</v>
       </c>
       <c r="E167" s="10" t="s">
-        <v>515</v>
+        <v>500</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -5323,7 +5323,7 @@
         <v>280</v>
       </c>
       <c r="E169" s="10" t="s">
-        <v>591</v>
+        <v>574</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -5340,7 +5340,7 @@
         <v>317</v>
       </c>
       <c r="E170" s="10" t="s">
-        <v>516</v>
+        <v>501</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -5348,10 +5348,10 @@
         <v>1</v>
       </c>
       <c r="C171" s="10" t="s">
-        <v>517</v>
+        <v>502</v>
       </c>
       <c r="D171" s="10" t="s">
-        <v>518</v>
+        <v>503</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -5368,7 +5368,7 @@
         <v>335</v>
       </c>
       <c r="E172" s="10" t="s">
-        <v>519</v>
+        <v>504</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="187">
@@ -5382,10 +5382,10 @@
         <v>326</v>
       </c>
       <c r="D173" s="10" t="s">
-        <v>559</v>
+        <v>542</v>
       </c>
       <c r="E173" s="11" t="s">
-        <v>560</v>
+        <v>543</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -5399,10 +5399,10 @@
         <v>337</v>
       </c>
       <c r="D174" s="10" t="s">
-        <v>520</v>
+        <v>505</v>
       </c>
       <c r="E174" s="10" t="s">
-        <v>521</v>
+        <v>506</v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -5416,10 +5416,10 @@
         <v>334</v>
       </c>
       <c r="D175" s="10" t="s">
-        <v>522</v>
+        <v>507</v>
       </c>
       <c r="E175" s="10" t="s">
-        <v>523</v>
+        <v>508</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -5436,7 +5436,7 @@
         <v>332</v>
       </c>
       <c r="E176" s="10" t="s">
-        <v>524</v>
+        <v>509</v>
       </c>
     </row>
     <row r="177" spans="1:6">
@@ -5453,7 +5453,7 @@
         <v>330</v>
       </c>
       <c r="E177" s="10" t="s">
-        <v>525</v>
+        <v>510</v>
       </c>
     </row>
     <row r="178" spans="1:6">
@@ -5467,10 +5467,10 @@
         <v>327</v>
       </c>
       <c r="D178" s="10" t="s">
-        <v>593</v>
+        <v>576</v>
       </c>
       <c r="E178" s="10" t="s">
-        <v>592</v>
+        <v>575</v>
       </c>
     </row>
     <row r="179" spans="1:6">
@@ -5487,7 +5487,7 @@
         <v>328</v>
       </c>
       <c r="E179" s="10" t="s">
-        <v>594</v>
+        <v>577</v>
       </c>
     </row>
     <row r="180" spans="1:6">
@@ -5501,10 +5501,10 @@
         <v>338</v>
       </c>
       <c r="D180" s="10" t="s">
-        <v>526</v>
+        <v>511</v>
       </c>
       <c r="E180" s="10" t="s">
-        <v>527</v>
+        <v>512</v>
       </c>
     </row>
     <row r="181" spans="1:6">
@@ -5512,10 +5512,10 @@
         <v>1</v>
       </c>
       <c r="C181" s="10" t="s">
-        <v>528</v>
+        <v>513</v>
       </c>
       <c r="D181" s="10" t="s">
-        <v>529</v>
+        <v>514</v>
       </c>
     </row>
     <row r="182" spans="1:6">
@@ -5529,10 +5529,10 @@
         <v>340</v>
       </c>
       <c r="D182" s="10" t="s">
-        <v>530</v>
+        <v>515</v>
       </c>
       <c r="E182" s="10" t="s">
-        <v>595</v>
+        <v>578</v>
       </c>
     </row>
     <row r="183" spans="1:6">
@@ -5546,10 +5546,10 @@
         <v>341</v>
       </c>
       <c r="D183" s="10" t="s">
-        <v>531</v>
+        <v>516</v>
       </c>
       <c r="E183" s="10" t="s">
-        <v>596</v>
+        <v>579</v>
       </c>
       <c r="F183" s="12"/>
     </row>
@@ -5564,10 +5564,10 @@
         <v>339</v>
       </c>
       <c r="D184" s="10" t="s">
-        <v>532</v>
+        <v>517</v>
       </c>
       <c r="E184" s="10" t="s">
-        <v>533</v>
+        <v>518</v>
       </c>
       <c r="F184" s="12"/>
     </row>
@@ -5585,7 +5585,7 @@
         <v>342</v>
       </c>
       <c r="E185" s="10" t="s">
-        <v>534</v>
+        <v>519</v>
       </c>
     </row>
     <row r="186" spans="1:6">
@@ -5593,10 +5593,10 @@
         <v>1</v>
       </c>
       <c r="C186" s="10" t="s">
-        <v>535</v>
+        <v>520</v>
       </c>
       <c r="D186" s="10" t="s">
-        <v>536</v>
+        <v>521</v>
       </c>
     </row>
     <row r="187" spans="1:6">
@@ -5610,10 +5610,10 @@
         <v>353</v>
       </c>
       <c r="D187" s="10" t="s">
-        <v>537</v>
+        <v>522</v>
       </c>
       <c r="E187" s="10" t="s">
-        <v>597</v>
+        <v>580</v>
       </c>
     </row>
     <row r="188" spans="1:6">
@@ -5630,7 +5630,7 @@
         <v>354</v>
       </c>
       <c r="E188" s="10" t="s">
-        <v>598</v>
+        <v>581</v>
       </c>
     </row>
     <row r="189" spans="1:6">
@@ -5644,10 +5644,10 @@
         <v>344</v>
       </c>
       <c r="D189" s="10" t="s">
-        <v>538</v>
+        <v>604</v>
       </c>
       <c r="E189" s="10" t="s">
-        <v>539</v>
+        <v>603</v>
       </c>
     </row>
     <row r="190" spans="1:6">
@@ -5661,7 +5661,7 @@
         <v>351</v>
       </c>
       <c r="D190" s="10" t="s">
-        <v>540</v>
+        <v>523</v>
       </c>
       <c r="E190" s="10" t="s">
         <v>350</v>
@@ -5698,7 +5698,7 @@
         <v>348</v>
       </c>
       <c r="E192" s="10" t="s">
-        <v>541</v>
+        <v>524</v>
       </c>
     </row>
     <row r="193" spans="1:5">
@@ -5715,7 +5715,7 @@
         <v>356</v>
       </c>
       <c r="E193" s="10" t="s">
-        <v>542</v>
+        <v>525</v>
       </c>
     </row>
     <row r="194" spans="1:5">
@@ -5729,10 +5729,10 @@
         <v>352</v>
       </c>
       <c r="D194" s="10" t="s">
-        <v>543</v>
+        <v>526</v>
       </c>
       <c r="E194" s="10" t="s">
-        <v>544</v>
+        <v>527</v>
       </c>
     </row>
     <row r="195" spans="1:5">
@@ -5740,10 +5740,10 @@
         <v>1</v>
       </c>
       <c r="C195" s="10" t="s">
-        <v>545</v>
+        <v>528</v>
       </c>
       <c r="D195" s="10" t="s">
-        <v>546</v>
+        <v>529</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -5760,7 +5760,7 @@
         <v>358</v>
       </c>
       <c r="E196" s="10" t="s">
-        <v>547</v>
+        <v>530</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -5777,7 +5777,7 @@
         <v>360</v>
       </c>
       <c r="E197" s="10" t="s">
-        <v>548</v>
+        <v>531</v>
       </c>
     </row>
     <row r="198" spans="1:5">

</xml_diff>